<commit_message>
remove hunting adult 3/5
</commit_message>
<xml_diff>
--- a/data/input/hunting_scenarios_abs.xlsx
+++ b/data/input/hunting_scenarios_abs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9690" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9696"/>
   </bookViews>
   <sheets>
     <sheet name="N" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="7">
   <si>
     <t>juvenileF</t>
   </si>
@@ -36,19 +36,13 @@
     <t>yearlingM</t>
   </si>
   <si>
-    <t>adult3F</t>
+    <t>Population</t>
   </si>
   <si>
-    <t>adult5F</t>
+    <t>adultF</t>
   </si>
   <si>
-    <t>adult3M</t>
-  </si>
-  <si>
-    <t>adult5M</t>
-  </si>
-  <si>
-    <t>Population</t>
+    <t>adultM</t>
   </si>
 </sst>
 </file>
@@ -376,23 +370,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
@@ -406,14 +400,8 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>0</v>
       </c>
@@ -432,14 +420,8 @@
       <c r="G2">
         <v>0</v>
       </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>0</v>
-      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>0</v>
       </c>
@@ -458,14 +440,8 @@
       <c r="G3">
         <v>0</v>
       </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>0</v>
-      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>0</v>
       </c>
@@ -484,14 +460,8 @@
       <c r="G4">
         <v>0</v>
       </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>0</v>
-      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>0</v>
       </c>
@@ -510,14 +480,8 @@
       <c r="G5">
         <v>0</v>
       </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>0</v>
-      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>0</v>
       </c>
@@ -536,14 +500,8 @@
       <c r="G6">
         <v>0</v>
       </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>0</v>
-      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>0</v>
       </c>
@@ -562,14 +520,8 @@
       <c r="G7">
         <v>0</v>
       </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>0</v>
-      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>0</v>
       </c>
@@ -588,14 +540,8 @@
       <c r="G8">
         <v>0</v>
       </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>0</v>
-      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>0</v>
       </c>
@@ -614,14 +560,8 @@
       <c r="G9">
         <v>0</v>
       </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>0</v>
-      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>0</v>
       </c>
@@ -640,14 +580,8 @@
       <c r="G10">
         <v>0</v>
       </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>0</v>
-      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>0</v>
       </c>
@@ -666,14 +600,8 @@
       <c r="G11">
         <v>0</v>
       </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>0</v>
-      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>0</v>
       </c>
@@ -692,14 +620,8 @@
       <c r="G12">
         <v>0</v>
       </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>0</v>
-      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>0</v>
       </c>
@@ -716,9 +638,6 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
         <v>0</v>
       </c>
     </row>
@@ -729,23 +648,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
@@ -759,14 +678,8 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>5</v>
-      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>5</v>
       </c>
@@ -785,14 +698,8 @@
       <c r="G2">
         <v>5</v>
       </c>
-      <c r="H2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>5</v>
-      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>5</v>
       </c>
@@ -811,14 +718,8 @@
       <c r="G3">
         <v>5</v>
       </c>
-      <c r="H3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>5</v>
-      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>5</v>
       </c>
@@ -837,14 +738,8 @@
       <c r="G4">
         <v>5</v>
       </c>
-      <c r="H4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>5</v>
-      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>5</v>
       </c>
@@ -863,14 +758,8 @@
       <c r="G5">
         <v>5</v>
       </c>
-      <c r="H5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>5</v>
       </c>
@@ -889,14 +778,8 @@
       <c r="G6">
         <v>5</v>
       </c>
-      <c r="H6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>5</v>
       </c>
@@ -915,14 +798,8 @@
       <c r="G7">
         <v>5</v>
       </c>
-      <c r="H7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>5</v>
-      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>5</v>
       </c>
@@ -941,14 +818,8 @@
       <c r="G8">
         <v>5</v>
       </c>
-      <c r="H8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>5</v>
-      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>5</v>
       </c>
@@ -967,14 +838,8 @@
       <c r="G9">
         <v>5</v>
       </c>
-      <c r="H9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>5</v>
-      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>5</v>
       </c>
@@ -993,14 +858,8 @@
       <c r="G10">
         <v>5</v>
       </c>
-      <c r="H10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>5</v>
-      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>5</v>
       </c>
@@ -1019,14 +878,8 @@
       <c r="G11">
         <v>5</v>
       </c>
-      <c r="H11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>5</v>
-      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>5</v>
       </c>
@@ -1045,14 +898,8 @@
       <c r="G12">
         <v>5</v>
       </c>
-      <c r="H12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>5</v>
-      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>5</v>
       </c>
@@ -1071,46 +918,35 @@
       <c r="G13">
         <v>5</v>
       </c>
-      <c r="H13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <f>SUM(A2:A13)</f>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <f>SUM(B2:B13)</f>
         <v>60</v>
       </c>
-      <c r="B16">
-        <f t="shared" ref="B16:H16" si="0">SUM(B2:B13)</f>
+      <c r="C16">
+        <f t="shared" ref="C16:G16" si="0">SUM(C2:C13)</f>
         <v>60</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="G16">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="H16">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="J16">
-        <f>SUM(A16:H16)</f>
-        <v>480</v>
+      <c r="I16">
+        <f>SUM(B16:G16)</f>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -1120,23 +956,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
@@ -1150,14 +986,8 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>5</v>
-      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>5</v>
       </c>
@@ -1176,14 +1006,8 @@
       <c r="G2">
         <v>5</v>
       </c>
-      <c r="H2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>5</v>
-      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>5</v>
       </c>
@@ -1202,14 +1026,8 @@
       <c r="G3">
         <v>5</v>
       </c>
-      <c r="H3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>5</v>
-      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>5</v>
       </c>
@@ -1228,14 +1046,8 @@
       <c r="G4">
         <v>5</v>
       </c>
-      <c r="H4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>5</v>
-      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>5</v>
       </c>
@@ -1254,21 +1066,15 @@
       <c r="G5">
         <v>5</v>
       </c>
-      <c r="H5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <f t="shared" ref="A6:F13" si="0">A$17</f>
-        <v>0</v>
-      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B6:F13" si="0">B$17</f>
         <v>0</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -1284,21 +1090,15 @@
       <c r="G6">
         <v>5</v>
       </c>
-      <c r="H6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -1314,21 +1114,15 @@
       <c r="G7">
         <v>5</v>
       </c>
-      <c r="H7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -1344,21 +1138,15 @@
       <c r="G8">
         <v>5</v>
       </c>
-      <c r="H8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="D9">
         <v>5</v>
@@ -1374,21 +1162,15 @@
       <c r="G9">
         <v>5</v>
       </c>
-      <c r="H9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -1404,21 +1186,15 @@
       <c r="G10">
         <v>5</v>
       </c>
-      <c r="H10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C11">
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="D11">
         <v>5</v>
@@ -1434,21 +1210,15 @@
       <c r="G11">
         <v>5</v>
       </c>
-      <c r="H11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="D12">
         <v>5</v>
@@ -1464,21 +1234,15 @@
       <c r="G12">
         <v>5</v>
       </c>
-      <c r="H12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C13">
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="D13">
         <v>5</v>
@@ -1494,22 +1258,15 @@
       <c r="G13">
         <v>5</v>
       </c>
-      <c r="H13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <f>SUM(A2:A13)</f>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <f>SUM(B2:B13)</f>
         <v>20</v>
       </c>
-      <c r="B16">
-        <f t="shared" ref="B16:H16" si="1">SUM(B2:B13)</f>
+      <c r="C16">
+        <f t="shared" ref="C16:G16" si="1">SUM(C2:C13)</f>
         <v>20</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="1"/>
-        <v>60</v>
       </c>
       <c r="D16">
         <f t="shared" si="1"/>
@@ -1527,13 +1284,9 @@
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="H16">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-      <c r="J16">
-        <f>SUM(A16:H16)</f>
-        <v>320</v>
+      <c r="I16">
+        <f>SUM(B16:G16)</f>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -1543,20 +1296,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1565,25 +1318,19 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2">
         <v>5</v>
@@ -1592,25 +1339,19 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <v>2</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>5</v>
-      </c>
-      <c r="I2">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3">
         <v>5</v>
@@ -1619,25 +1360,19 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>5</v>
-      </c>
-      <c r="I3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4">
         <v>5</v>
@@ -1646,25 +1381,19 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>5</v>
-      </c>
-      <c r="I4">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5">
         <v>5</v>
@@ -1673,25 +1402,19 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E5">
         <v>2</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>5</v>
-      </c>
-      <c r="I5">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6">
         <v>5</v>
@@ -1700,25 +1423,19 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E6">
         <v>2</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>5</v>
-      </c>
-      <c r="I6">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7">
         <v>5</v>
@@ -1727,25 +1444,19 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E7">
         <v>2</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>5</v>
-      </c>
-      <c r="I7">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8">
         <v>5</v>
@@ -1754,25 +1465,19 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E8">
         <v>2</v>
       </c>
       <c r="F8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>5</v>
-      </c>
-      <c r="I8">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9">
         <v>5</v>
@@ -1781,25 +1486,19 @@
         <v>1</v>
       </c>
       <c r="D9">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E9">
         <v>2</v>
       </c>
       <c r="F9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>5</v>
-      </c>
-      <c r="I9">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10">
         <v>5</v>
@@ -1808,25 +1507,19 @@
         <v>1</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E10">
         <v>2</v>
       </c>
       <c r="F10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>5</v>
-      </c>
-      <c r="I10">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11">
         <v>5</v>
@@ -1835,25 +1528,19 @@
         <v>1</v>
       </c>
       <c r="D11">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E11">
         <v>2</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>5</v>
-      </c>
-      <c r="I11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12">
         <v>5</v>
@@ -1862,25 +1549,19 @@
         <v>1</v>
       </c>
       <c r="D12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E12">
         <v>2</v>
       </c>
       <c r="F12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>5</v>
-      </c>
-      <c r="I12">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13">
         <v>5</v>
@@ -1889,36 +1570,30 @@
         <v>1</v>
       </c>
       <c r="D13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E13">
         <v>2</v>
       </c>
       <c r="F13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13">
-        <v>5</v>
-      </c>
-      <c r="I13">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16">
         <f>SUM(B2:B13)</f>
         <v>60</v>
       </c>
       <c r="C16">
-        <f t="shared" ref="C16:I16" si="0">SUM(C2:C13)</f>
+        <f t="shared" ref="C16:G16" si="0">SUM(C2:C13)</f>
         <v>12</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
@@ -1926,23 +1601,15 @@
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="G16">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="H16">
-        <f t="shared" si="0"/>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="I16">
-        <f t="shared" si="0"/>
-        <v>120</v>
-      </c>
-      <c r="K16">
-        <f>SUM(B16:I16)</f>
-        <v>372</v>
+        <f>SUM(B16:G16)</f>
+        <v>252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>